<commit_message>
part 6 in prog
</commit_message>
<xml_diff>
--- a/results/runtimes.xlsx
+++ b/results/runtimes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley\Documents\ECE522\mp4\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE402F4A-0B93-4D60-A32A-10913D2F9420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115C17DD-3629-4087-87E9-93457E13EDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="part4" sheetId="1" r:id="rId1"/>
     <sheet name="part5" sheetId="2" r:id="rId2"/>
+    <sheet name="part6" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>Ideal-1024</t>
   </si>
@@ -118,6 +119,27 @@
   </si>
   <si>
     <t>Perf Ratios</t>
+  </si>
+  <si>
+    <t>Bert-base</t>
+  </si>
+  <si>
+    <t>InceptionV3-base</t>
+  </si>
+  <si>
+    <t>ResNet152-base</t>
+  </si>
+  <si>
+    <t>SENet154-base</t>
+  </si>
+  <si>
+    <t>VIT-base</t>
+  </si>
+  <si>
+    <t>Perf Ratio</t>
+  </si>
+  <si>
+    <t>BASED ON GPU-CPU-SSD, REPLACING SSD WITH CXL</t>
   </si>
 </sst>
 </file>
@@ -172,21 +194,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -497,15 +516,15 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="B1:E1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.53515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.4609375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -530,17 +549,17 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>20928839517</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>20928839517</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>41857679034</v>
       </c>
       <c r="E2" t="b">
-        <f t="shared" ref="E2:E16" si="0">IF((B2+C2)=D2,TRUE,FALSE)</f>
+        <f t="shared" ref="E2:E29" si="0">IF((B2+C2)=D2,TRUE,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -548,13 +567,13 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>71175129375</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>71175129375</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>142350258750</v>
       </c>
       <c r="E3" t="b">
@@ -566,13 +585,13 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>133443504591</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>133443504591</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>266887009182</v>
       </c>
       <c r="E4" t="b">
@@ -584,13 +603,13 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>159444569683</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>159444569683</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>318889139366</v>
       </c>
       <c r="E5" t="b">
@@ -602,13 +621,13 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>3919374526</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>3919374526</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>7838749052</v>
       </c>
       <c r="E6" t="b">
@@ -665,13 +684,13 @@
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>141569826941</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>123579302542</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>265149129483</v>
       </c>
       <c r="E11" t="b">
@@ -683,13 +702,13 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>142970763281</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>139989684384</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>282960447665</v>
       </c>
       <c r="E12" t="b">
@@ -701,13 +720,13 @@
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>264240683726</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>257545901189</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>521786584915</v>
       </c>
       <c r="E13" t="b">
@@ -719,13 +738,13 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>477608372101</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>468562902391</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <v>946171274492</v>
       </c>
       <c r="E14" t="b">
@@ -737,13 +756,13 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>40612521647</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>36107617197</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>76720138844</v>
       </c>
       <c r="E15" t="b">
@@ -773,6 +792,10 @@
       <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E17" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
@@ -787,6 +810,10 @@
       <c r="D18" s="1">
         <v>756207488146</v>
       </c>
+      <c r="E18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
@@ -801,6 +828,10 @@
       <c r="D19" s="1">
         <v>622560940893</v>
       </c>
+      <c r="E19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
@@ -815,6 +846,10 @@
       <c r="D20" s="1">
         <v>1146350248020</v>
       </c>
+      <c r="E20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
@@ -829,6 +864,10 @@
       <c r="D21" s="1">
         <v>2052273624486</v>
       </c>
+      <c r="E21" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
@@ -842,12 +881,20 @@
       </c>
       <c r="D22" s="1">
         <v>340826045176</v>
+      </c>
+      <c r="E22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
+      <c r="E23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
@@ -862,6 +909,10 @@
       <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E24" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
@@ -876,6 +927,10 @@
       <c r="D25" s="1">
         <v>41857679034</v>
       </c>
+      <c r="E25" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
@@ -890,6 +945,10 @@
       <c r="D26" s="1">
         <v>278569841106</v>
       </c>
+      <c r="E26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
@@ -904,6 +963,10 @@
       <c r="D27" s="1">
         <v>490068800624</v>
       </c>
+      <c r="E27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
@@ -918,6 +981,10 @@
       <c r="D28" s="1">
         <v>2052273624486</v>
       </c>
+      <c r="E28" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
@@ -931,6 +998,10 @@
       </c>
       <c r="D29" s="1">
         <v>43196724241</v>
+      </c>
+      <c r="E29" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -964,13 +1035,13 @@
       <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="3">
         <v>131986612062</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <v>112266689356</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="3">
         <v>244253301418</v>
       </c>
       <c r="E32" t="b">
@@ -982,13 +1053,13 @@
       <c r="A33" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="3">
         <v>142970763281</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="3">
         <v>139989684384</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="3">
         <v>282960447665</v>
       </c>
       <c r="E33" t="b">
@@ -1000,13 +1071,13 @@
       <c r="A34" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="3">
         <v>251655078132</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <v>244319509089</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="3">
         <v>495974587221</v>
       </c>
       <c r="E34" t="b">
@@ -1018,13 +1089,13 @@
       <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="3">
         <v>466228995826</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="3">
         <v>456431950066</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="3">
         <v>922660945892</v>
       </c>
       <c r="E35" t="b">
@@ -1036,13 +1107,13 @@
       <c r="A36" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="3">
         <v>25313940949</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="3">
         <v>21454177966</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="3">
         <v>46768118915</v>
       </c>
       <c r="E36" t="b">
@@ -1059,35 +1130,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD371E-8240-4966-B6E6-5EDF76D71DAC}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24.921875" customWidth="1"/>
-    <col min="2" max="2" width="17.23046875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.69140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.61328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.23046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.69140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.61328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1095,13 +1166,13 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <v>40612521647</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>36107617197</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>76720138844</v>
       </c>
       <c r="E2" t="b">
@@ -1113,13 +1184,13 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="2">
         <v>39530287905</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <v>36781860777</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="2">
         <v>76312148682</v>
       </c>
       <c r="E3" t="b">
@@ -1135,13 +1206,13 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>41226710353</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>37349960758</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
         <v>78576671111</v>
       </c>
       <c r="E4" t="b">
@@ -1162,13 +1233,13 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="2">
         <v>142970763281</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>139989684384</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>282960447665</v>
       </c>
       <c r="E9" t="b">
@@ -1180,13 +1251,13 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="2">
         <v>123953535953</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>122545884391</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="2">
         <v>246499420344</v>
       </c>
       <c r="E10" t="b">
@@ -1202,13 +1273,13 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="2">
         <v>141569826941</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>123579302542</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="2">
         <v>265149129483</v>
       </c>
       <c r="E11" t="b">
@@ -1220,13 +1291,13 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="2">
         <v>141569826941</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <v>123579302542</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="2">
         <v>265149129483</v>
       </c>
       <c r="E12" t="b">
@@ -1242,13 +1313,13 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="2">
         <v>264240683726</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="2">
         <v>257545901189</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="2">
         <v>521786584915</v>
       </c>
       <c r="E13" t="b">
@@ -1260,13 +1331,13 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="2">
         <v>264240683726</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="2">
         <v>257545901189</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="2">
         <v>521786584915</v>
       </c>
       <c r="E14" t="b">
@@ -1282,13 +1353,13 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="2">
         <v>477608372101</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="2">
         <v>468562902391</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="2">
         <v>946171274492</v>
       </c>
       <c r="E15" t="b">
@@ -1300,13 +1371,13 @@
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="2">
         <v>477608372101</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="2">
         <v>468562902391</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="2">
         <v>946171274492</v>
       </c>
       <c r="E16" t="b">
@@ -1322,4 +1393,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909E0C75-3972-44E8-B6C8-7388D620E6B9}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.61328125" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.53515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3">
+        <v>131986612062</v>
+      </c>
+      <c r="C3" s="3">
+        <v>112266689356</v>
+      </c>
+      <c r="D3" s="3">
+        <v>244253301418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>126175516592</v>
+      </c>
+      <c r="C4" s="2">
+        <v>112266689356</v>
+      </c>
+      <c r="D4" s="2">
+        <v>238442205948</v>
+      </c>
+      <c r="E4" t="b">
+        <f>IF(C4+B4=D4,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>D3/D4</f>
+        <v>1.024371085844036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3">
+        <v>142970763281</v>
+      </c>
+      <c r="C5" s="3">
+        <v>139989684384</v>
+      </c>
+      <c r="D5" s="3">
+        <v>282960447665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>144700567589</v>
+      </c>
+      <c r="C6" s="2">
+        <v>139989684384</v>
+      </c>
+      <c r="D6" s="2">
+        <v>284690251973</v>
+      </c>
+      <c r="E6" t="b">
+        <f t="shared" ref="E6:E12" si="0">IF(C6+B6=D6,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f>D5/D6</f>
+        <v>0.99392390748888704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3">
+        <v>251655078132</v>
+      </c>
+      <c r="C7" s="3">
+        <v>244319509089</v>
+      </c>
+      <c r="D7" s="3">
+        <v>495974587221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>256372356123</v>
+      </c>
+      <c r="C8" s="2">
+        <v>244319509089</v>
+      </c>
+      <c r="D8" s="2">
+        <v>500691865212</v>
+      </c>
+      <c r="E8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>D7/D8</f>
+        <v>0.99057848086067335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3">
+        <v>466228995826</v>
+      </c>
+      <c r="C9" s="3">
+        <v>456431950066</v>
+      </c>
+      <c r="D9" s="3">
+        <v>922660945892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>471919199046</v>
+      </c>
+      <c r="C10" s="2">
+        <v>456431950066</v>
+      </c>
+      <c r="D10" s="2">
+        <v>928351149112</v>
+      </c>
+      <c r="E10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>D9/D10</f>
+        <v>0.99387063480726778</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3">
+        <v>25313940949</v>
+      </c>
+      <c r="C11" s="3">
+        <v>21454177966</v>
+      </c>
+      <c r="D11" s="3">
+        <v>46768118915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <v>23629607726</v>
+      </c>
+      <c r="C12" s="2">
+        <v>21454177966</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45083785692</v>
+      </c>
+      <c r="E12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f>D11/D12</f>
+        <v>1.0373600663109106</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>